<commit_message>
minor data type files
</commit_message>
<xml_diff>
--- a/dist/rd3.2.0-beta-0.9.2.xlsx
+++ b/dist/rd3.2.0-beta-0.9.2.xlsx
@@ -43,7 +43,7 @@
     <t>RD3 Variants</t>
   </si>
   <si>
-    <t>Solve-RD RD3 database(v2.0-beta-0.9.2, 2022-10-07)</t>
+    <t>Solve-RD RD3 database (v2.0-beta-0.9.2, 2022-10-07)</t>
   </si>
   <si>
     <t>Information about RD3 Releases, Studies, Cohorts, Collaborators, etc.</t>
@@ -154,19 +154,19 @@
     <t>variantinfo</t>
   </si>
   <si>
-    <t>SolveRD Subjects</t>
-  </si>
-  <si>
-    <t>SolveRD Subject Information</t>
-  </si>
-  <si>
-    <t>SolveRD Samples</t>
-  </si>
-  <si>
-    <t>Solve RD Experiments</t>
-  </si>
-  <si>
-    <t>SolveRD Files</t>
+    <t>Solve-RD Subjects</t>
+  </si>
+  <si>
+    <t>Solve-RD Subject Information</t>
+  </si>
+  <si>
+    <t>Solve-RD Samples</t>
+  </si>
+  <si>
+    <t>Solve-RD Experiments</t>
+  </si>
+  <si>
+    <t>Solve-RD Files</t>
   </si>
   <si>
     <t>Cohorts</t>
@@ -1762,334 +1762,334 @@
     <t>rangeMax</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C172217</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C63536</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42883</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_000087</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/SCDO_0002829</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ExO_0000127</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C47824</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C61512</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/ExO_0000127</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C63536</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C172217</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/SCDO_0002829</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_000087</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25461</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171105</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C15607</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25412</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25461</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C15607</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171105</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42883</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C47824</t>
+    <t>http://purl.obolibrary.org/obo/GSSO_001755</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16735</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C67073</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42775</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000100</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176375</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C115505</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C166209</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171191</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16977</t>
+  </si>
+  <si>
+    <t>https://w3id.org/reproduceme#wasUpdatedBy</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93495</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/SNOMEDCT/423493009</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142702</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142704</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIT_0004546</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C19924</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70713</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_3273</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25173</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C47922</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C94324</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C40974</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C40975</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25737</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_001330</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16493</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GO_0001894</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
+  </si>
+  <si>
+    <t>http://www.orpha.net/ORDO/Orphanet_C023</t>
+  </si>
+  <si>
+    <t>https://w3id.org/reproduceme#doi</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C69208</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000037</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C83164</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C135383</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C153145</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001891</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/RO_0000056</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DUO_0000001</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93400</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0001094</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171337</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ICO_0000178</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/FIX_0000704</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C40976</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171276</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_000669</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000035</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_000670</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/HL7/C0442737</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C64917</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C166237</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C43361</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C127771</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176373</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000006</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C53190</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/efo/EFO_0005518</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C183337</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C90353</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0500027</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0001921</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_001083</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93629</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C89336</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171103</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25393</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C89336</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/DUO_0000001</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIT_0004546</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C94324</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C67073</t>
-  </si>
-  <si>
-    <t>http://www.ebi.ac.uk/efo/EFO_0005518</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C47922</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25173</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C153145</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171276</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/RO_0000056</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000100</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0001891</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C40976</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C40975</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000006</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16735</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0001921</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C103264</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C127771</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_001083</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142704</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93629</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0001094</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C176373</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/ICO_0000178</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C135383</t>
-  </si>
-  <si>
-    <t>https://w3id.org/reproduceme#doi</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171191</t>
-  </si>
-  <si>
-    <t>https://w3id.org/reproduceme#wasUpdatedBy</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16977</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142702</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93400</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C171252</t>
   </si>
   <si>
-    <t>http://semanticscience.org/resource/SIO_000670</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C69208</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/HL7/C0442737</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C43361</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000035</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93495</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C90353</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_000669</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C115505</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/FIX_0000704</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C166209</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171103</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C64917</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C19924</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_001330</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/SNOMEDCT/423493009</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0500027</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GO_0001894</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C176375</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C53190</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000037</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/data_3273</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42775</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C183337</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C83164</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25737</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C166237</t>
-  </si>
-  <si>
-    <t>http://www.orpha.net/ORDO/Orphanet_C023</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70713</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16493</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171337</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C40974</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GSSO_001755</t>
-  </si>
-  <si>
     <t>NCIT</t>
   </si>
   <si>
+    <t>SIO</t>
+  </si>
+  <si>
+    <t>SCDO</t>
+  </si>
+  <si>
     <t>ExO</t>
   </si>
   <si>
-    <t>SCDO</t>
-  </si>
-  <si>
-    <t>SIO</t>
+    <t>GSSO</t>
+  </si>
+  <si>
+    <t>OMIABIS</t>
+  </si>
+  <si>
+    <t>reproduceme</t>
+  </si>
+  <si>
+    <t>SNOMEDCT</t>
+  </si>
+  <si>
+    <t>OMIT</t>
+  </si>
+  <si>
+    <t>EDAM</t>
+  </si>
+  <si>
+    <t>GO</t>
+  </si>
+  <si>
+    <t>Orphanet</t>
+  </si>
+  <si>
+    <t>OBI</t>
+  </si>
+  <si>
+    <t>RO</t>
   </si>
   <si>
     <t>DUO</t>
   </si>
   <si>
-    <t>OMIT</t>
+    <t>GENEPIO</t>
+  </si>
+  <si>
+    <t>ICO</t>
+  </si>
+  <si>
+    <t>FIX</t>
+  </si>
+  <si>
+    <t>HL7</t>
   </si>
   <si>
     <t>EFO</t>
-  </si>
-  <si>
-    <t>RO</t>
-  </si>
-  <si>
-    <t>OMIABIS</t>
-  </si>
-  <si>
-    <t>OBI</t>
-  </si>
-  <si>
-    <t>GENEPIO</t>
-  </si>
-  <si>
-    <t>ICO</t>
-  </si>
-  <si>
-    <t>reproduceme</t>
-  </si>
-  <si>
-    <t>HL7</t>
-  </si>
-  <si>
-    <t>FIX</t>
-  </si>
-  <si>
-    <t>SNOMEDCT</t>
-  </si>
-  <si>
-    <t>GO</t>
-  </si>
-  <si>
-    <t>EDAM</t>
-  </si>
-  <si>
-    <t>Orphanet</t>
-  </si>
-  <si>
-    <t>GSSO</t>
   </si>
   <si>
     <t>isAssociatedWith</t>
@@ -12691,10 +12691,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>581</v>
@@ -12711,16 +12711,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>582</v>
       </c>
       <c r="D3" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E3" t="s">
         <v>691</v>
@@ -12731,10 +12731,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>583</v>
@@ -12751,16 +12751,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>584</v>
       </c>
       <c r="D5" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="E5" t="s">
         <v>691</v>
@@ -12791,10 +12791,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>586</v>
@@ -12811,10 +12811,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>587</v>
@@ -12831,10 +12831,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>588</v>
@@ -12851,10 +12851,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>589</v>
@@ -12891,10 +12891,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>591</v>
@@ -12911,10 +12911,10 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>592</v>
@@ -12931,16 +12931,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>457</v>
+        <v>502</v>
       </c>
       <c r="B14" t="s">
-        <v>457</v>
+        <v>502</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>593</v>
       </c>
       <c r="D14" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
       <c r="E14" t="s">
         <v>691</v>
@@ -12951,10 +12951,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="B15" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>594</v>
@@ -12971,10 +12971,10 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>499</v>
+        <v>471</v>
       </c>
       <c r="B16" t="s">
-        <v>499</v>
+        <v>471</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>595</v>
@@ -12991,16 +12991,16 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>494</v>
+        <v>506</v>
       </c>
       <c r="B17" t="s">
-        <v>494</v>
+        <v>506</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>596</v>
       </c>
       <c r="D17" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="E17" t="s">
         <v>691</v>
@@ -13011,10 +13011,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>463</v>
+        <v>486</v>
       </c>
       <c r="B18" t="s">
-        <v>463</v>
+        <v>486</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>597</v>
@@ -13031,10 +13031,10 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>444</v>
+        <v>515</v>
       </c>
       <c r="B19" t="s">
-        <v>444</v>
+        <v>515</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>598</v>
@@ -13051,10 +13051,10 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>471</v>
+        <v>493</v>
       </c>
       <c r="B20" t="s">
-        <v>471</v>
+        <v>493</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>599</v>
@@ -13071,16 +13071,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>469</v>
+        <v>484</v>
       </c>
       <c r="B21" t="s">
-        <v>469</v>
+        <v>484</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>600</v>
       </c>
       <c r="D21" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="E21" t="s">
         <v>691</v>
@@ -13091,10 +13091,10 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="B22" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>601</v>
@@ -13111,10 +13111,10 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>442</v>
+        <v>477</v>
       </c>
       <c r="B23" t="s">
-        <v>442</v>
+        <v>477</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>602</v>
@@ -13131,10 +13131,10 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>520</v>
+        <v>446</v>
       </c>
       <c r="B24" t="s">
-        <v>520</v>
+        <v>446</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>603</v>
@@ -13151,16 +13151,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>478</v>
+        <v>456</v>
       </c>
       <c r="B25" t="s">
-        <v>478</v>
+        <v>456</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>604</v>
       </c>
       <c r="D25" t="s">
-        <v>671</v>
+        <v>677</v>
       </c>
       <c r="E25" t="s">
         <v>691</v>
@@ -13171,16 +13171,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>448</v>
+        <v>483</v>
       </c>
       <c r="B26" t="s">
-        <v>448</v>
+        <v>483</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>605</v>
       </c>
       <c r="D26" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="E26" t="s">
         <v>691</v>
@@ -13191,16 +13191,16 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>486</v>
+        <v>461</v>
       </c>
       <c r="B27" t="s">
-        <v>486</v>
+        <v>461</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>606</v>
       </c>
       <c r="D27" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E27" t="s">
         <v>691</v>
@@ -13211,10 +13211,10 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>441</v>
+        <v>518</v>
       </c>
       <c r="B28" t="s">
-        <v>441</v>
+        <v>518</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>607</v>
@@ -13231,16 +13231,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>474</v>
+        <v>516</v>
       </c>
       <c r="B29" t="s">
-        <v>474</v>
+        <v>516</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>608</v>
       </c>
       <c r="D29" t="s">
-        <v>680</v>
+        <v>671</v>
       </c>
       <c r="E29" t="s">
         <v>691</v>
@@ -13251,10 +13251,10 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="B30" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>609</v>
@@ -13271,16 +13271,16 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
       <c r="B31" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>610</v>
       </c>
       <c r="D31" t="s">
-        <v>671</v>
+        <v>679</v>
       </c>
       <c r="E31" t="s">
         <v>691</v>
@@ -13291,10 +13291,10 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>505</v>
+        <v>513</v>
       </c>
       <c r="B32" t="s">
-        <v>505</v>
+        <v>513</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>611</v>
@@ -13311,10 +13311,10 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>484</v>
+        <v>468</v>
       </c>
       <c r="B33" t="s">
-        <v>484</v>
+        <v>468</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>612</v>
@@ -13331,16 +13331,16 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>510</v>
+        <v>490</v>
       </c>
       <c r="B34" t="s">
-        <v>510</v>
+        <v>490</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>613</v>
       </c>
       <c r="D34" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="E34" t="s">
         <v>691</v>
@@ -13357,7 +13357,7 @@
         <v>115</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
       <c r="D35" t="s">
         <v>671</v>
@@ -13371,16 +13371,16 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>449</v>
+        <v>464</v>
       </c>
       <c r="B36" t="s">
-        <v>449</v>
+        <v>464</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>614</v>
       </c>
       <c r="D36" t="s">
-        <v>671</v>
+        <v>680</v>
       </c>
       <c r="E36" t="s">
         <v>691</v>
@@ -13391,16 +13391,16 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>475</v>
+        <v>442</v>
       </c>
       <c r="B37" t="s">
-        <v>475</v>
+        <v>442</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>615</v>
       </c>
       <c r="D37" t="s">
-        <v>681</v>
+        <v>671</v>
       </c>
       <c r="E37" t="s">
         <v>691</v>
@@ -13411,10 +13411,10 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>470</v>
+        <v>481</v>
       </c>
       <c r="B38" t="s">
-        <v>470</v>
+        <v>481</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>616</v>
@@ -13431,10 +13431,10 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>467</v>
+        <v>497</v>
       </c>
       <c r="B39" t="s">
-        <v>467</v>
+        <v>497</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>617</v>
@@ -13451,16 +13451,16 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>491</v>
+        <v>444</v>
       </c>
       <c r="B40" t="s">
-        <v>491</v>
+        <v>444</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>618</v>
       </c>
       <c r="D40" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="E40" t="s">
         <v>691</v>
@@ -13471,10 +13471,10 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="B41" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>619</v>
@@ -13491,10 +13491,10 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>455</v>
+        <v>505</v>
       </c>
       <c r="B42" t="s">
-        <v>455</v>
+        <v>505</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>620</v>
@@ -13511,10 +13511,10 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>497</v>
+        <v>451</v>
       </c>
       <c r="B43" t="s">
-        <v>497</v>
+        <v>451</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>621</v>
@@ -13531,16 +13531,16 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="B44" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>622</v>
       </c>
       <c r="D44" t="s">
-        <v>681</v>
+        <v>672</v>
       </c>
       <c r="E44" t="s">
         <v>691</v>
@@ -13551,10 +13551,10 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>514</v>
+        <v>492</v>
       </c>
       <c r="B45" t="s">
-        <v>514</v>
+        <v>492</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>623</v>
@@ -13571,16 +13571,16 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>450</v>
+        <v>466</v>
       </c>
       <c r="B46" t="s">
-        <v>450</v>
+        <v>466</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>624</v>
       </c>
       <c r="D46" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E46" t="s">
         <v>691</v>
@@ -13591,10 +13591,10 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="B47" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>625</v>
@@ -13611,16 +13611,16 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>507</v>
+        <v>113</v>
       </c>
       <c r="B48" t="s">
-        <v>507</v>
+        <v>113</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>626</v>
+        <v>581</v>
       </c>
       <c r="D48" t="s">
-        <v>683</v>
+        <v>671</v>
       </c>
       <c r="E48" t="s">
         <v>691</v>
@@ -13631,13 +13631,13 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>477</v>
+        <v>454</v>
       </c>
       <c r="B49" t="s">
-        <v>477</v>
+        <v>454</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D49" t="s">
         <v>671</v>
@@ -13651,16 +13651,16 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>456</v>
+        <v>499</v>
       </c>
       <c r="B50" t="s">
-        <v>456</v>
+        <v>499</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D50" t="s">
-        <v>683</v>
+        <v>671</v>
       </c>
       <c r="E50" t="s">
         <v>691</v>
@@ -13671,16 +13671,16 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>446</v>
+        <v>460</v>
       </c>
       <c r="B51" t="s">
-        <v>446</v>
+        <v>460</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D51" t="s">
-        <v>671</v>
+        <v>682</v>
       </c>
       <c r="E51" t="s">
         <v>691</v>
@@ -13691,16 +13691,16 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="B52" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D52" t="s">
-        <v>671</v>
+        <v>677</v>
       </c>
       <c r="E52" t="s">
         <v>691</v>
@@ -13711,13 +13711,13 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B53" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D53" t="s">
         <v>671</v>
@@ -13731,16 +13731,16 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>472</v>
+        <v>511</v>
       </c>
       <c r="B54" t="s">
-        <v>472</v>
+        <v>511</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D54" t="s">
-        <v>671</v>
+        <v>676</v>
       </c>
       <c r="E54" t="s">
         <v>691</v>
@@ -13751,13 +13751,13 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>479</v>
+        <v>458</v>
       </c>
       <c r="B55" t="s">
-        <v>479</v>
+        <v>458</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D55" t="s">
         <v>671</v>
@@ -13771,16 +13771,16 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>496</v>
+        <v>459</v>
       </c>
       <c r="B56" t="s">
-        <v>496</v>
+        <v>459</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D56" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="E56" t="s">
         <v>691</v>
@@ -13791,13 +13791,13 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>487</v>
+        <v>520</v>
       </c>
       <c r="B57" t="s">
-        <v>487</v>
+        <v>520</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>588</v>
+        <v>634</v>
       </c>
       <c r="D57" t="s">
         <v>671</v>
@@ -13811,16 +13811,16 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>517</v>
+        <v>474</v>
       </c>
       <c r="B58" t="s">
-        <v>517</v>
+        <v>474</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>635</v>
       </c>
       <c r="D58" t="s">
-        <v>671</v>
+        <v>683</v>
       </c>
       <c r="E58" t="s">
         <v>691</v>
@@ -13831,10 +13831,10 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B59" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>636</v>
@@ -13851,13 +13851,13 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>473</v>
+        <v>112</v>
       </c>
       <c r="B60" t="s">
-        <v>473</v>
+        <v>112</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>637</v>
+        <v>588</v>
       </c>
       <c r="D60" t="s">
         <v>671</v>
@@ -13871,16 +13871,16 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="B61" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D61" t="s">
-        <v>671</v>
+        <v>685</v>
       </c>
       <c r="E61" t="s">
         <v>691</v>
@@ -13891,16 +13891,16 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>488</v>
+        <v>498</v>
       </c>
       <c r="B62" t="s">
-        <v>488</v>
+        <v>498</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D62" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="E62" t="s">
         <v>691</v>
@@ -13911,13 +13911,13 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
       <c r="B63" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D63" t="s">
         <v>671</v>
@@ -13931,16 +13931,16 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B64" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D64" t="s">
-        <v>671</v>
+        <v>686</v>
       </c>
       <c r="E64" t="s">
         <v>691</v>
@@ -13951,16 +13951,16 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="B65" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D65" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="E65" t="s">
         <v>691</v>
@@ -13971,13 +13971,13 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
       <c r="B66" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D66" t="s">
         <v>671</v>
@@ -13991,16 +13991,16 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>476</v>
+        <v>450</v>
       </c>
       <c r="B67" t="s">
-        <v>476</v>
+        <v>450</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D67" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="E67" t="s">
         <v>691</v>
@@ -14011,16 +14011,16 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="B68" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D68" t="s">
-        <v>671</v>
+        <v>688</v>
       </c>
       <c r="E68" t="s">
         <v>691</v>
@@ -14031,13 +14031,13 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>485</v>
+        <v>509</v>
       </c>
       <c r="B69" t="s">
-        <v>485</v>
+        <v>509</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D69" t="s">
         <v>671</v>
@@ -14051,13 +14051,13 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>112</v>
+        <v>478</v>
       </c>
       <c r="B70" t="s">
-        <v>112</v>
+        <v>478</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>581</v>
+        <v>646</v>
       </c>
       <c r="D70" t="s">
         <v>671</v>
@@ -14071,16 +14071,16 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>519</v>
+        <v>495</v>
       </c>
       <c r="B71" t="s">
-        <v>519</v>
+        <v>495</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>647</v>
       </c>
       <c r="D71" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="E71" t="s">
         <v>691</v>
@@ -14091,10 +14091,10 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="B72" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>648</v>
@@ -14111,16 +14111,16 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>501</v>
+        <v>488</v>
       </c>
       <c r="B73" t="s">
-        <v>501</v>
+        <v>488</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
       <c r="D73" t="s">
-        <v>671</v>
+        <v>676</v>
       </c>
       <c r="E73" t="s">
         <v>691</v>
@@ -14131,16 +14131,16 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>513</v>
+        <v>496</v>
       </c>
       <c r="B74" t="s">
-        <v>513</v>
+        <v>496</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="D74" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="E74" t="s">
         <v>691</v>
@@ -14151,16 +14151,16 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>113</v>
+        <v>447</v>
       </c>
       <c r="B75" t="s">
-        <v>113</v>
+        <v>447</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>584</v>
+        <v>651</v>
       </c>
       <c r="D75" t="s">
-        <v>671</v>
+        <v>689</v>
       </c>
       <c r="E75" t="s">
         <v>691</v>
@@ -14171,16 +14171,16 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="B76" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="D76" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="E76" t="s">
         <v>691</v>
@@ -14191,16 +14191,16 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>461</v>
+        <v>504</v>
       </c>
       <c r="B77" t="s">
-        <v>461</v>
+        <v>504</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="D77" t="s">
-        <v>686</v>
+        <v>671</v>
       </c>
       <c r="E77" t="s">
         <v>691</v>
@@ -14211,16 +14211,16 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>512</v>
+        <v>473</v>
       </c>
       <c r="B78" t="s">
-        <v>512</v>
+        <v>473</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="D78" t="s">
-        <v>680</v>
+        <v>671</v>
       </c>
       <c r="E78" t="s">
         <v>691</v>
@@ -14231,16 +14231,16 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B79" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="D79" t="s">
-        <v>687</v>
+        <v>671</v>
       </c>
       <c r="E79" t="s">
         <v>691</v>
@@ -14251,13 +14251,13 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>515</v>
+        <v>120</v>
       </c>
       <c r="B80" t="s">
-        <v>515</v>
+        <v>120</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>654</v>
+        <v>591</v>
       </c>
       <c r="D80" t="s">
         <v>671</v>
@@ -14271,10 +14271,10 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>120</v>
+        <v>487</v>
       </c>
       <c r="B81" t="s">
-        <v>120</v>
+        <v>487</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>589</v>
@@ -14291,13 +14291,13 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>489</v>
+        <v>514</v>
       </c>
       <c r="B82" t="s">
-        <v>489</v>
+        <v>514</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="D82" t="s">
         <v>671</v>
@@ -14311,16 +14311,16 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B83" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="D83" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="E83" t="s">
         <v>691</v>
@@ -14331,16 +14331,16 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>464</v>
+        <v>482</v>
       </c>
       <c r="B84" t="s">
-        <v>464</v>
+        <v>482</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>657</v>
+        <v>641</v>
       </c>
       <c r="D84" t="s">
-        <v>688</v>
+        <v>671</v>
       </c>
       <c r="E84" t="s">
         <v>691</v>
@@ -14351,10 +14351,10 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>506</v>
+        <v>489</v>
       </c>
       <c r="B85" t="s">
-        <v>506</v>
+        <v>489</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>658</v>
@@ -14371,16 +14371,16 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>508</v>
+        <v>469</v>
       </c>
       <c r="B86" t="s">
-        <v>508</v>
+        <v>469</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>659</v>
       </c>
       <c r="D86" t="s">
-        <v>671</v>
+        <v>690</v>
       </c>
       <c r="E86" t="s">
         <v>691</v>
@@ -14391,10 +14391,10 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>458</v>
+        <v>508</v>
       </c>
       <c r="B87" t="s">
-        <v>458</v>
+        <v>508</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>660</v>
@@ -14411,10 +14411,10 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>498</v>
+        <v>465</v>
       </c>
       <c r="B88" t="s">
-        <v>498</v>
+        <v>465</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>661</v>
@@ -14431,16 +14431,16 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>451</v>
+        <v>512</v>
       </c>
       <c r="B89" t="s">
-        <v>451</v>
+        <v>512</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>662</v>
       </c>
       <c r="D89" t="s">
-        <v>671</v>
+        <v>683</v>
       </c>
       <c r="E89" t="s">
         <v>691</v>
@@ -14451,16 +14451,16 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>453</v>
+        <v>475</v>
       </c>
       <c r="B90" t="s">
-        <v>453</v>
+        <v>475</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>663</v>
       </c>
       <c r="D90" t="s">
-        <v>671</v>
+        <v>686</v>
       </c>
       <c r="E90" t="s">
         <v>691</v>
@@ -14471,16 +14471,16 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>504</v>
+        <v>491</v>
       </c>
       <c r="B91" t="s">
-        <v>504</v>
+        <v>491</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>664</v>
       </c>
       <c r="D91" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="E91" t="s">
         <v>691</v>
@@ -14491,16 +14491,16 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="B92" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>665</v>
       </c>
       <c r="D92" t="s">
-        <v>689</v>
+        <v>671</v>
       </c>
       <c r="E92" t="s">
         <v>691</v>
@@ -14511,10 +14511,10 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>468</v>
+        <v>443</v>
       </c>
       <c r="B93" t="s">
-        <v>468</v>
+        <v>443</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>666</v>
@@ -14531,10 +14531,10 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>492</v>
+        <v>519</v>
       </c>
       <c r="B94" t="s">
-        <v>492</v>
+        <v>519</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>667</v>
@@ -14551,10 +14551,10 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>480</v>
+        <v>457</v>
       </c>
       <c r="B95" t="s">
-        <v>480</v>
+        <v>457</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>668</v>
@@ -14571,10 +14571,10 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>503</v>
+        <v>470</v>
       </c>
       <c r="B96" t="s">
-        <v>503</v>
+        <v>470</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>669</v>
@@ -14591,16 +14591,16 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>502</v>
+        <v>479</v>
       </c>
       <c r="B97" t="s">
-        <v>502</v>
+        <v>479</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>670</v>
       </c>
       <c r="D97" t="s">
-        <v>690</v>
+        <v>671</v>
       </c>
       <c r="E97" t="s">
         <v>691</v>
@@ -14657,7 +14657,7 @@
     <hyperlink ref="F23" r:id="rId44" location="isAssociatedWith"/>
     <hyperlink ref="C24" r:id="rId45"/>
     <hyperlink ref="F24" r:id="rId46" location="isAssociatedWith"/>
-    <hyperlink ref="C25" r:id="rId47"/>
+    <hyperlink ref="C25" r:id="rId47" location="wasUpdatedBy"/>
     <hyperlink ref="F25" r:id="rId48" location="isAssociatedWith"/>
     <hyperlink ref="C26" r:id="rId49"/>
     <hyperlink ref="F26" r:id="rId50" location="isAssociatedWith"/>
@@ -14703,15 +14703,15 @@
     <hyperlink ref="F46" r:id="rId90" location="isAssociatedWith"/>
     <hyperlink ref="C47" r:id="rId91"/>
     <hyperlink ref="F47" r:id="rId92" location="isAssociatedWith"/>
-    <hyperlink ref="C48" r:id="rId93" location="doi"/>
+    <hyperlink ref="C48" r:id="rId93"/>
     <hyperlink ref="F48" r:id="rId94" location="isAssociatedWith"/>
     <hyperlink ref="C49" r:id="rId95"/>
     <hyperlink ref="F49" r:id="rId96" location="isAssociatedWith"/>
-    <hyperlink ref="C50" r:id="rId97" location="wasUpdatedBy"/>
+    <hyperlink ref="C50" r:id="rId97"/>
     <hyperlink ref="F50" r:id="rId98" location="isAssociatedWith"/>
     <hyperlink ref="C51" r:id="rId99"/>
     <hyperlink ref="F51" r:id="rId100" location="isAssociatedWith"/>
-    <hyperlink ref="C52" r:id="rId101"/>
+    <hyperlink ref="C52" r:id="rId101" location="doi"/>
     <hyperlink ref="F52" r:id="rId102" location="isAssociatedWith"/>
     <hyperlink ref="C53" r:id="rId103"/>
     <hyperlink ref="F53" r:id="rId104" location="isAssociatedWith"/>

</xml_diff>